<commit_message>
Tijd tot KBS les 2
</commit_message>
<xml_diff>
--- a/KBS-M1_Tijdschrijfformulier.xlsx
+++ b/KBS-M1_Tijdschrijfformulier.xlsx
@@ -5,27 +5,27 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alwin\Documents\GitHub\KBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruud Louwerse\Documents\School\Semester 1\KBS\github\KBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23250" windowHeight="13170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Projectlid1" sheetId="7" r:id="rId1"/>
-    <sheet name="Projectlid2" sheetId="8" r:id="rId2"/>
+    <sheet name="Alwin Eizema" sheetId="7" r:id="rId1"/>
+    <sheet name="Ruud Louwerse" sheetId="8" r:id="rId2"/>
     <sheet name="Projectlid3" sheetId="9" r:id="rId3"/>
     <sheet name="Projectlid4" sheetId="10" r:id="rId4"/>
     <sheet name="Projectlid5" sheetId="11" r:id="rId5"/>
     <sheet name="Projectlid6" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Projectlid1!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Projectlid2!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Alwin Eizema'!$A$1:$D$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Projectlid3!$A$1:$D$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Projectlid4!$A$1:$D$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Projectlid5!$A$1:$D$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Projectlid6!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Ruud Louwerse'!$A$1:$D$47</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>ICTm1m</t>
+  </si>
+  <si>
+    <t>Ruud Louwerse</t>
+  </si>
+  <si>
+    <t>ICTM1M</t>
+  </si>
+  <si>
+    <t>Kickoff KBS</t>
   </si>
 </sst>
 </file>
@@ -192,9 +201,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -288,7 +297,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -610,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,16 +793,25 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -804,7 +822,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -816,7 +834,7 @@
       </c>
       <c r="B7">
         <f>252-(SUM(C10:C152)/60)</f>
-        <v>252</v>
+        <v>247.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -837,6 +855,30 @@
       </c>
       <c r="D9" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1338,6 +1380,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008036A50752E2824D899ADB653A634107" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2de00fd1d47445d7b69804c94a655239">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fd18b65b941b90f0796ec8ea2bab88d" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1480,16 +1532,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1500,6 +1542,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F02D2AB-3A08-4775-83FF-70C9E461BFAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1518,23 +1577,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
   <ds:schemaRefs>

</xml_diff>